<commit_message>
Updated all the files for mergre
</commit_message>
<xml_diff>
--- a/com.airbnb/src/test/resources/TestData.xlsx
+++ b/com.airbnb/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Team1BootCamp\com.airbnb\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8259915F-B174-4669-BFF5-5AC59C335295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7526BAF2-0311-4753-BF29-701F312EC7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="7" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="8" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="FooterTitle" sheetId="23" r:id="rId1"/>
@@ -20,8 +20,8 @@
     <sheet name="Support" sheetId="27" r:id="rId5"/>
     <sheet name="FutureGateway" sheetId="28" r:id="rId6"/>
     <sheet name="ArtsCulture" sheetId="30" r:id="rId7"/>
-    <sheet name="Count" sheetId="31" r:id="rId8"/>
-    <sheet name="OutdoorAdventure" sheetId="29" r:id="rId9"/>
+    <sheet name="OutdoorAdventure" sheetId="29" r:id="rId8"/>
+    <sheet name="Count" sheetId="31" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="239">
   <si>
     <t>How Airbnb works</t>
   </si>
@@ -738,6 +738,27 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>185</t>
   </si>
 </sst>
 </file>
@@ -817,7 +838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -845,6 +866,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1519,7 +1541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481660E0-8DDC-4945-B474-6B233162C7A0}">
   <dimension ref="A1:A87"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A78" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
@@ -1964,31 +1986,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2836EF-9BA6-4742-B604-E03B8C1E33B0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092AE368-E522-439E-91D3-7D0E10B8D68F}">
   <dimension ref="A1:A185"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A165" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -2923,4 +2924,99 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2836EF-9BA6-4742-B604-E03B8C1E33B0}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="11"/>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="11"/>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="11"/>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="11"/>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="11"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="11"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="11"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>